<commit_message>
Fixing SCD0263 and SCD0267
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0263 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0263 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7476C975-39A8-4FA6-A65D-494C3AE30192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845EB39A-0D6B-4B59-A378-09F9D9485509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +184,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -205,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -226,6 +233,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +558,7 @@
     <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -629,7 +640,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="9">
-        <v>39237</v>
+        <v>35758</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -642,13 +653,13 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="9">
-        <v>9418305324</v>
+        <v>9720826341</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="9">
-        <v>9721622304</v>
+      <c r="O2" s="11">
+        <v>9669179367</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="4"/>
@@ -671,8 +682,8 @@
       <c r="E3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9">
-        <v>29637</v>
+      <c r="F3" s="10">
+        <v>35795</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>9</v>
@@ -704,7 +715,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="9">
-        <v>39237</v>
+        <v>35758</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>9</v>
@@ -723,13 +734,13 @@
         <v>23</v>
       </c>
       <c r="M4" s="9">
-        <v>9418305324</v>
+        <v>9720826341</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="9">
-        <v>9721622304</v>
+      <c r="O4" s="11">
+        <v>9669179367</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="2"/>
@@ -751,7 +762,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="9">
-        <v>23948</v>
+        <v>19256</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>9</v>
@@ -789,7 +800,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="9">
-        <v>39237</v>
+        <v>35758</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>9</v>
@@ -808,13 +819,13 @@
         <v>23</v>
       </c>
       <c r="M6" s="9">
-        <v>9418305324</v>
+        <v>9720826341</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="9">
-        <v>9721622304</v>
+      <c r="O6" s="11">
+        <v>9669179367</v>
       </c>
       <c r="P6" s="8"/>
     </row>
@@ -835,7 +846,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="9">
-        <v>19256</v>
+        <v>23948</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>9</v>
@@ -864,7 +875,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="9">
-        <v>39237</v>
+        <v>35758</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>9</v>
@@ -883,13 +894,13 @@
         <v>23</v>
       </c>
       <c r="M8" s="9">
-        <v>9418305324</v>
+        <v>9720826341</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="9">
-        <v>9721622304</v>
+      <c r="O8" s="11">
+        <v>9669179367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>